<commit_message>
match up with nlp-core and fastner upgrade to 1.1.1
</commit_message>
<xml_diff>
--- a/conf/rush_rules_v3.xlsx
+++ b/conf/rush_rules_v3.xlsx
@@ -2686,8 +2686,8 @@
   </sheetPr>
   <dimension ref="A1:D955"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A236" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A256" activeCellId="0" sqref="A256"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A315" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A334" activeCellId="0" sqref="A334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>